<commit_message>
More last last minute changes (sigh).
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
+++ b/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
@@ -721,7 +721,7 @@
   <dimension ref="A1:B65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -760,7 +760,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>